<commit_message>
Updated Switchboard - pull down resistors, fixed routing, protection diodes and different battery connector
</commit_message>
<xml_diff>
--- a/src/schematics/ScouseTom_SwitchNetwork/Gerber/SwitchBoard_Pick_and_Place.xlsx
+++ b/src/schematics/ScouseTom_SwitchNetwork/Gerber/SwitchBoard_Pick_and_Place.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="SwitchBoard" localSheetId="0">Sheet1!$A$2:$F$58</definedName>
-    <definedName name="SwitchBoard_1" localSheetId="0">Sheet1!$A$59:$F$75</definedName>
+    <definedName name="SwitchBoard_1" localSheetId="0">Sheet1!$A$2:$F$71</definedName>
+    <definedName name="SwitchBoard_2" localSheetId="0">Sheet1!$A$72:$F$90</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -25,7 +25,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="SwitchBoard" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\Jimbles\Copy\ScouseTom\src\schematics\ScouseTom_SwitchNetwork\Gerber\SwitchBoard.mnt" tab="0" space="1" consecutive="1">
+    <textPr codePage="437" sourceFile="C:\Users\Jimbles\ScouseTom\src\schematics\ScouseTom_SwitchNetwork\Gerber\SwitchBoard.mnt" tab="0" space="1" consecutive="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -37,7 +37,7 @@
     </textPr>
   </connection>
   <connection id="2" name="SwitchBoard1" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="437" sourceFile="C:\Users\Jimbles\Copy\ScouseTom\src\schematics\ScouseTom_SwitchNetwork\Gerber\SwitchBoard.mnb" tab="0" space="1" consecutive="1">
+    <textPr codePage="437" sourceFile="C:\Users\Jimbles\ScouseTom\src\schematics\ScouseTom_SwitchNetwork\Gerber\SwitchBoard.mnb" tab="0" space="1" consecutive="1">
       <textFields count="6">
         <textField/>
         <textField/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="143">
   <si>
     <t>Ref Des</t>
   </si>
@@ -366,81 +366,9 @@
     <t>X1</t>
   </si>
   <si>
-    <t>MC0805X106K6R3CT</t>
-  </si>
-  <si>
-    <t>MC0805B104K500CT</t>
-  </si>
-  <si>
     <t>Top</t>
   </si>
   <si>
-    <t>MC0805B225K250CT</t>
-  </si>
-  <si>
-    <t>293D107X9010C2TE3</t>
-  </si>
-  <si>
-    <t>MC0805B103K500CT</t>
-  </si>
-  <si>
-    <t>MC0805B105K250CT</t>
-  </si>
-  <si>
-    <t>KPT-2012YC</t>
-  </si>
-  <si>
-    <t>KPT-2012CGCK</t>
-  </si>
-  <si>
-    <t>KPT-2012EC</t>
-  </si>
-  <si>
-    <t>MC01W08051470R</t>
-  </si>
-  <si>
-    <t>MC01W080511K</t>
-  </si>
-  <si>
-    <t>MC01W080512K</t>
-  </si>
-  <si>
-    <t>MC01W080512M00</t>
-  </si>
-  <si>
-    <t>MC01W08051360K</t>
-  </si>
-  <si>
-    <t>MC01W080511M80</t>
-  </si>
-  <si>
-    <t>MC01W08051820K</t>
-  </si>
-  <si>
-    <t>MC01W0805147K</t>
-  </si>
-  <si>
-    <t>MC01W08051470K</t>
-  </si>
-  <si>
-    <t>MC01W0805110K</t>
-  </si>
-  <si>
-    <t>MC01W0805110M0</t>
-  </si>
-  <si>
-    <t>BC807-40,215</t>
-  </si>
-  <si>
-    <t>MCP73831T-2ACI/OT</t>
-  </si>
-  <si>
-    <t>TPS61090RSARG4</t>
-  </si>
-  <si>
-    <t>USB3070-30-A</t>
-  </si>
-  <si>
     <t>C6</t>
   </si>
   <si>
@@ -495,19 +423,64 @@
     <t>Bottom</t>
   </si>
   <si>
-    <t>JP3</t>
-  </si>
-  <si>
-    <t>LiPo</t>
-  </si>
-  <si>
-    <t>JST-2-SMD</t>
-  </si>
-  <si>
     <t>MOLEX_47346-0001</t>
   </si>
   <si>
-    <t>S2B-PH-SM4-TB(LF)(SN)</t>
+    <t>R25</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>R26</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R32</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>R34</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>1N4148W-7-F</t>
+  </si>
+  <si>
+    <t>SOD123</t>
+  </si>
+  <si>
+    <t>D2</t>
   </si>
 </sst>
 </file>
@@ -1010,38 +983,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1192,11 +1139,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SwitchBoard" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SwitchBoard_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SwitchBoard_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SwitchBoard_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1486,47 +1433,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H75"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="50" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="G1" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="38" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1549,11 +1496,9 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>104</v>
-      </c>
+      <c r="G2" s="2"/>
       <c r="H2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1575,11 +1520,9 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>104</v>
-      </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1601,11 +1544,9 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>104</v>
-      </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1627,11 +1568,9 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="G5" s="33"/>
       <c r="H5" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1653,11 +1592,9 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="G6" s="33"/>
       <c r="H6" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1679,11 +1616,9 @@
       <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>105</v>
-      </c>
+      <c r="G7" s="33"/>
       <c r="H7" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1705,11 +1640,9 @@
       <c r="F8" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>107</v>
-      </c>
+      <c r="G8" s="11"/>
       <c r="H8" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1731,11 +1664,9 @@
       <c r="F9" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>108</v>
-      </c>
+      <c r="G9" s="21"/>
       <c r="H9" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1757,11 +1688,9 @@
       <c r="F10" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>104</v>
-      </c>
+      <c r="G10" s="2"/>
       <c r="H10" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1783,11 +1712,9 @@
       <c r="F11" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>105</v>
-      </c>
+      <c r="G11" s="33"/>
       <c r="H11" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -1809,11 +1736,9 @@
       <c r="F12" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="11" t="s">
-        <v>109</v>
-      </c>
+      <c r="G12" s="11"/>
       <c r="H12" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1835,11 +1760,9 @@
       <c r="F13" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>108</v>
-      </c>
+      <c r="G13" s="21"/>
       <c r="H13" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1861,11 +1784,9 @@
       <c r="F14" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="10" t="s">
-        <v>105</v>
-      </c>
+      <c r="G14" s="33"/>
       <c r="H14" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1887,11 +1808,9 @@
       <c r="F15" t="s">
         <v>10</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>105</v>
-      </c>
+      <c r="G15" s="33"/>
       <c r="H15" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1913,11 +1832,9 @@
       <c r="F16" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>110</v>
-      </c>
+      <c r="G16" s="33"/>
       <c r="H16" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1939,11 +1856,9 @@
       <c r="F17" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>105</v>
-      </c>
+      <c r="G17" s="33"/>
       <c r="H17" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1965,11 +1880,9 @@
       <c r="F18" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="12" t="s">
-        <v>110</v>
-      </c>
+      <c r="G18" s="33"/>
       <c r="H18" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1991,11 +1904,9 @@
       <c r="F19" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="12" t="s">
-        <v>105</v>
-      </c>
+      <c r="G19" s="33"/>
       <c r="H19" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2017,11 +1928,9 @@
       <c r="F20" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="13" t="s">
-        <v>105</v>
-      </c>
+      <c r="G20" s="33"/>
       <c r="H20" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2043,11 +1952,9 @@
       <c r="F21" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="13" t="s">
-        <v>110</v>
-      </c>
+      <c r="G21" s="33"/>
       <c r="H21" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2069,11 +1976,9 @@
       <c r="F22" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="13" t="s">
-        <v>105</v>
-      </c>
+      <c r="G22" s="33"/>
       <c r="H22" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2095,103 +2000,95 @@
       <c r="F23" t="s">
         <v>10</v>
       </c>
-      <c r="G23" s="13" t="s">
-        <v>110</v>
-      </c>
+      <c r="G23" s="33"/>
       <c r="H23" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>147</v>
+        <v>39</v>
       </c>
       <c r="B24">
-        <v>-5.08</v>
+        <v>8.26</v>
       </c>
       <c r="C24">
-        <v>91.61</v>
+        <v>95.89</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E24" t="s">
-        <v>148</v>
+        <v>40</v>
       </c>
       <c r="F24" t="s">
-        <v>149</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>151</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="G24" s="21"/>
       <c r="H24" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B25">
-        <v>8.26</v>
+        <v>-15.24</v>
       </c>
       <c r="C25">
-        <v>95.89</v>
+        <v>76.2</v>
       </c>
       <c r="D25">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E25" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>94</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="G25" s="12"/>
       <c r="H25" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B26">
         <v>-15.24</v>
       </c>
       <c r="C26">
-        <v>76.2</v>
+        <v>73.66</v>
       </c>
       <c r="D26">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F26" t="s">
         <v>44</v>
       </c>
-      <c r="G26" s="15" t="s">
-        <v>111</v>
-      </c>
+      <c r="G26" s="12"/>
       <c r="H26" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B27">
         <v>-15.24</v>
       </c>
       <c r="C27">
-        <v>73.66</v>
+        <v>94.62</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E27" t="s">
         <v>46</v>
@@ -2199,149 +2096,137 @@
       <c r="F27" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="15" t="s">
-        <v>112</v>
-      </c>
+      <c r="G27" s="12"/>
       <c r="H27" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B28">
         <v>-15.24</v>
       </c>
       <c r="C28">
-        <v>94.62</v>
+        <v>88.9</v>
       </c>
       <c r="D28">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F28" t="s">
         <v>44</v>
       </c>
-      <c r="G28" s="15" t="s">
-        <v>112</v>
-      </c>
+      <c r="G28" s="12"/>
       <c r="H28" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B29">
-        <v>-15.24</v>
+        <v>-5.71</v>
       </c>
       <c r="C29">
-        <v>88.9</v>
+        <v>76.2</v>
       </c>
       <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29" t="s">
-        <v>49</v>
+        <v>180</v>
+      </c>
+      <c r="E29">
+        <v>470</v>
       </c>
       <c r="F29" t="s">
-        <v>44</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>113</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G29" s="3"/>
       <c r="H29" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B30">
         <v>-5.71</v>
       </c>
       <c r="C30">
-        <v>76.2</v>
+        <v>74.099999999999994</v>
       </c>
       <c r="D30">
         <v>180</v>
       </c>
-      <c r="E30">
-        <v>470</v>
+      <c r="E30" t="s">
+        <v>53</v>
       </c>
       <c r="F30" t="s">
         <v>51</v>
       </c>
-      <c r="G30" s="16" t="s">
-        <v>114</v>
-      </c>
+      <c r="G30" s="4"/>
       <c r="H30" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B31">
-        <v>-5.71</v>
+        <v>-5.08</v>
       </c>
       <c r="C31">
-        <v>74.099999999999994</v>
+        <v>78.739999999999995</v>
       </c>
       <c r="D31">
         <v>180</v>
       </c>
       <c r="E31" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F31" t="s">
         <v>51</v>
       </c>
-      <c r="G31" s="17" t="s">
-        <v>115</v>
-      </c>
+      <c r="G31" s="5"/>
       <c r="H31" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B32">
-        <v>-5.08</v>
+        <v>10.79</v>
       </c>
       <c r="C32">
-        <v>78.739999999999995</v>
+        <v>78.11</v>
       </c>
       <c r="D32">
         <v>180</v>
       </c>
       <c r="E32" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F32" t="s">
         <v>51</v>
       </c>
-      <c r="G32" s="17" t="s">
-        <v>116</v>
-      </c>
+      <c r="G32" s="5"/>
       <c r="H32" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B33">
-        <v>10.79</v>
+        <v>15.88</v>
       </c>
       <c r="C33">
         <v>78.11</v>
@@ -2350,238 +2235,220 @@
         <v>180</v>
       </c>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F33" t="s">
         <v>51</v>
       </c>
-      <c r="G33" s="17" t="s">
-        <v>117</v>
-      </c>
+      <c r="G33" s="5"/>
       <c r="H33" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B34">
-        <v>15.88</v>
+        <v>17.14</v>
       </c>
       <c r="C34">
-        <v>78.11</v>
+        <v>84.45</v>
       </c>
       <c r="D34">
         <v>180</v>
       </c>
       <c r="E34" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F34" t="s">
         <v>51</v>
       </c>
-      <c r="G34" s="17" t="s">
-        <v>118</v>
-      </c>
+      <c r="G34" s="5"/>
       <c r="H34" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B35">
-        <v>17.14</v>
+        <v>20.64</v>
       </c>
       <c r="C35">
-        <v>84.45</v>
+        <v>83.12</v>
       </c>
       <c r="D35">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E35" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F35" t="s">
         <v>51</v>
       </c>
-      <c r="G35" s="18" t="s">
-        <v>119</v>
-      </c>
+      <c r="G35" s="6"/>
       <c r="H35" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B36">
-        <v>20.64</v>
+        <v>17.14</v>
       </c>
       <c r="C36">
-        <v>83.12</v>
+        <v>81.28</v>
       </c>
       <c r="D36">
         <v>90</v>
       </c>
       <c r="E36" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F36" t="s">
         <v>51</v>
       </c>
-      <c r="G36" s="18" t="s">
-        <v>120</v>
-      </c>
+      <c r="G36" s="6"/>
       <c r="H36" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B37">
-        <v>17.14</v>
+        <v>-11.43</v>
       </c>
       <c r="C37">
-        <v>81.28</v>
+        <v>93.34</v>
       </c>
       <c r="D37">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="E37" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
         <v>51</v>
       </c>
-      <c r="G37" s="18" t="s">
-        <v>117</v>
-      </c>
+      <c r="G37" s="6"/>
       <c r="H37" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B38">
-        <v>-11.43</v>
+        <v>10.16</v>
       </c>
       <c r="C38">
-        <v>93.34</v>
+        <v>75.56</v>
       </c>
       <c r="D38">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="E38" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F38" t="s">
         <v>51</v>
       </c>
-      <c r="G38" s="18" t="s">
-        <v>115</v>
-      </c>
+      <c r="G38" s="6"/>
       <c r="H38" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B39">
-        <v>10.16</v>
+        <v>6.99</v>
       </c>
       <c r="C39">
-        <v>75.56</v>
+        <v>76.84</v>
       </c>
       <c r="D39">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E39" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F39" t="s">
         <v>51</v>
       </c>
-      <c r="G39" s="20" t="s">
-        <v>121</v>
-      </c>
+      <c r="G39" s="8"/>
       <c r="H39" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B40">
-        <v>6.99</v>
+        <v>-11.43</v>
       </c>
       <c r="C40">
-        <v>76.84</v>
+        <v>88.9</v>
       </c>
       <c r="D40">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E40" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="F40" t="s">
         <v>51</v>
       </c>
-      <c r="G40" s="20" t="s">
-        <v>122</v>
-      </c>
+      <c r="G40" s="8"/>
       <c r="H40" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B41">
-        <v>-11.43</v>
+        <v>130.81</v>
       </c>
       <c r="C41">
-        <v>88.9</v>
+        <v>15.24</v>
       </c>
       <c r="D41">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="F41" t="s">
         <v>51</v>
       </c>
-      <c r="G41" s="20" t="s">
-        <v>115</v>
-      </c>
+      <c r="G41" s="8"/>
       <c r="H41" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B42">
         <v>130.81</v>
       </c>
       <c r="C42">
-        <v>15.24</v>
+        <v>45.09</v>
       </c>
       <c r="D42">
-        <v>270</v>
+        <v>90</v>
       </c>
       <c r="E42" t="s">
         <v>73</v>
@@ -2589,22 +2456,20 @@
       <c r="F42" t="s">
         <v>51</v>
       </c>
-      <c r="G42" s="19" t="s">
-        <v>123</v>
-      </c>
+      <c r="G42" s="7"/>
       <c r="H42" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B43">
         <v>130.81</v>
       </c>
       <c r="C43">
-        <v>45.09</v>
+        <v>72.39</v>
       </c>
       <c r="D43">
         <v>90</v>
@@ -2615,48 +2480,44 @@
       <c r="F43" t="s">
         <v>51</v>
       </c>
-      <c r="G43" s="21" t="s">
-        <v>123</v>
-      </c>
+      <c r="G43" s="9"/>
       <c r="H43" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B44">
-        <v>130.81</v>
+        <v>19.690000000000001</v>
       </c>
       <c r="C44">
-        <v>72.39</v>
+        <v>47.62</v>
       </c>
       <c r="D44">
         <v>90</v>
       </c>
       <c r="E44" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F44" t="s">
         <v>51</v>
       </c>
-      <c r="G44" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="G44" s="10"/>
       <c r="H44" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B45">
-        <v>19.690000000000001</v>
+        <v>16.510000000000002</v>
       </c>
       <c r="C45">
-        <v>47.62</v>
+        <v>45.09</v>
       </c>
       <c r="D45">
         <v>90</v>
@@ -2667,789 +2528,1071 @@
       <c r="F45" t="s">
         <v>51</v>
       </c>
-      <c r="G45" s="23" t="s">
-        <v>124</v>
-      </c>
+      <c r="G45" s="11"/>
       <c r="H45" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>124</v>
       </c>
       <c r="B46">
-        <v>16.510000000000002</v>
+        <v>-4.1900000000000004</v>
       </c>
       <c r="C46">
-        <v>45.09</v>
+        <v>45.72</v>
       </c>
       <c r="D46">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="E46" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F46" t="s">
-        <v>51</v>
-      </c>
-      <c r="G46" s="23" t="s">
-        <v>124</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G46" s="11"/>
       <c r="H46" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="B47">
-        <v>3.81</v>
+        <v>-1.1399999999999999</v>
       </c>
       <c r="C47">
-        <v>76.84</v>
+        <v>56.01</v>
       </c>
       <c r="D47">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F47" t="s">
-        <v>81</v>
-      </c>
-      <c r="G47" s="24" t="s">
         <v>125</v>
       </c>
+      <c r="G47" s="12"/>
       <c r="H47" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="B48">
-        <v>-5.08</v>
+        <v>-0.76</v>
       </c>
       <c r="C48">
-        <v>81.92</v>
+        <v>47.62</v>
       </c>
       <c r="D48">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E48" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F48" t="s">
-        <v>84</v>
-      </c>
-      <c r="G48" s="26" t="s">
-        <v>126</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G48" s="14"/>
       <c r="H48" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="B49">
-        <v>43.82</v>
+        <v>-4.95</v>
       </c>
       <c r="C49">
-        <v>61.6</v>
+        <v>64.77</v>
       </c>
       <c r="D49">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="E49" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F49" t="s">
-        <v>87</v>
-      </c>
-      <c r="G49" s="25" t="s">
-        <v>86</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G49" s="13"/>
       <c r="H49" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="B50">
-        <v>12.7</v>
+        <v>-2.54</v>
       </c>
       <c r="C50">
-        <v>83.19</v>
+        <v>62.99</v>
       </c>
       <c r="D50">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="E50" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F50" t="s">
-        <v>90</v>
-      </c>
-      <c r="G50" s="28" t="s">
-        <v>127</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G50" s="16"/>
       <c r="H50" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B51">
-        <v>43.81</v>
+        <v>-3.68</v>
       </c>
       <c r="C51">
-        <v>29.85</v>
+        <v>28.32</v>
       </c>
       <c r="D51">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E51" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F51" t="s">
-        <v>87</v>
-      </c>
-      <c r="G51" s="27" t="s">
-        <v>86</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G51" s="15"/>
       <c r="H51" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="B52">
-        <v>123.19</v>
+        <v>-5.08</v>
       </c>
       <c r="C52">
-        <v>22.23</v>
+        <v>51.44</v>
       </c>
       <c r="D52">
         <v>270</v>
       </c>
       <c r="E52" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F52" t="s">
-        <v>87</v>
-      </c>
-      <c r="G52" s="30" t="s">
-        <v>86</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G52" s="18"/>
       <c r="H52" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="B53">
-        <v>24.13</v>
+        <v>-3.81</v>
       </c>
       <c r="C53">
-        <v>91.44</v>
+        <v>57.28</v>
       </c>
       <c r="D53">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E53" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="F53" t="s">
-        <v>95</v>
-      </c>
-      <c r="G53" s="29" t="s">
-        <v>94</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G53" s="17"/>
       <c r="H53" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="B54">
-        <v>123.19</v>
+        <v>-3.68</v>
       </c>
       <c r="C54">
-        <v>50.17</v>
+        <v>26.92</v>
       </c>
       <c r="D54">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="E54" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F54" t="s">
-        <v>87</v>
-      </c>
-      <c r="G54" s="31" t="s">
-        <v>86</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G54" s="19"/>
       <c r="H54" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>134</v>
       </c>
       <c r="B55">
-        <v>6.99</v>
+        <v>-4.83</v>
       </c>
       <c r="C55">
-        <v>62.23</v>
+        <v>14.86</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E55" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="F55" t="s">
-        <v>99</v>
-      </c>
-      <c r="G55" s="32" t="s">
-        <v>98</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G55" s="20"/>
       <c r="H55" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="B56">
-        <v>123.19</v>
+        <v>-4.83</v>
       </c>
       <c r="C56">
-        <v>76.2</v>
+        <v>16.89</v>
       </c>
       <c r="D56">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="E56" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="F56" t="s">
-        <v>87</v>
-      </c>
-      <c r="G56" s="32" t="s">
-        <v>86</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="G56" s="20"/>
       <c r="H56" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" s="33">
-        <v>6.99</v>
-      </c>
-      <c r="C57" s="33">
-        <v>48.26</v>
-      </c>
-      <c r="D57" s="33">
-        <v>0</v>
-      </c>
-      <c r="E57" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="F57" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="G57" s="34" t="s">
-        <v>102</v>
-      </c>
+      <c r="A57" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="B57" s="21">
+        <v>-4.7</v>
+      </c>
+      <c r="C57" s="21">
+        <v>21.97</v>
+      </c>
+      <c r="D57" s="21">
+        <v>180</v>
+      </c>
+      <c r="E57" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F57" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="G57" s="22"/>
       <c r="H57" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="B58" s="33">
-        <v>-14.54</v>
-      </c>
-      <c r="C58" s="33">
-        <v>81.92</v>
-      </c>
-      <c r="D58" s="33">
-        <v>270</v>
-      </c>
-      <c r="E58" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="F58" s="33"/>
-      <c r="G58" s="35" t="s">
-        <v>128</v>
-      </c>
+      <c r="A58" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B58" s="21">
+        <v>-4.83</v>
+      </c>
+      <c r="C58" s="21">
+        <v>18.41</v>
+      </c>
+      <c r="D58" s="21">
+        <v>180</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F58" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="G58" s="23"/>
       <c r="H58" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="B59">
-        <v>41.28</v>
+        <v>-4.7</v>
       </c>
       <c r="C59">
-        <v>84.45</v>
+        <v>24.38</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="E59" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F59" t="s">
-        <v>10</v>
-      </c>
-      <c r="G59" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="H59" t="s">
-        <v>146</v>
+        <v>125</v>
+      </c>
+      <c r="G59" s="24"/>
+      <c r="H59" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="B60">
-        <v>41.28</v>
+        <v>3.81</v>
       </c>
       <c r="C60">
-        <v>53.98</v>
+        <v>76.84</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E60" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="F60" t="s">
-        <v>10</v>
-      </c>
-      <c r="G60" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="H60" s="33" t="s">
-        <v>146</v>
+        <v>81</v>
+      </c>
+      <c r="G60" s="25"/>
+      <c r="H60" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>131</v>
+        <v>82</v>
       </c>
       <c r="B61">
-        <v>126.37</v>
+        <v>-5.08</v>
       </c>
       <c r="C61">
-        <v>29.21</v>
+        <v>81.92</v>
       </c>
       <c r="D61">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E61" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="F61" t="s">
-        <v>10</v>
-      </c>
-      <c r="G61" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="H61" s="33" t="s">
-        <v>146</v>
+        <v>84</v>
+      </c>
+      <c r="G61" s="26"/>
+      <c r="H61" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>85</v>
       </c>
       <c r="B62">
-        <v>126.37</v>
+        <v>43.82</v>
       </c>
       <c r="C62">
-        <v>57.15</v>
+        <v>61.6</v>
       </c>
       <c r="D62">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E62" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="F62" t="s">
-        <v>10</v>
-      </c>
-      <c r="G62" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="H62" s="33" t="s">
-        <v>146</v>
+        <v>87</v>
+      </c>
+      <c r="G62" s="27"/>
+      <c r="H62" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>133</v>
+        <v>88</v>
       </c>
       <c r="B63">
-        <v>126.37</v>
+        <v>12.7</v>
       </c>
       <c r="C63">
-        <v>82.55</v>
+        <v>83.19</v>
       </c>
       <c r="D63">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="E63" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="F63" t="s">
-        <v>10</v>
-      </c>
-      <c r="G63" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="H63" s="33" t="s">
-        <v>146</v>
+        <v>90</v>
+      </c>
+      <c r="G63" s="28"/>
+      <c r="H63" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
       <c r="B64">
-        <v>37.47</v>
+        <v>43.81</v>
       </c>
       <c r="C64">
-        <v>64.77</v>
+        <v>29.85</v>
       </c>
       <c r="D64">
         <v>90</v>
       </c>
       <c r="E64" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="F64" t="s">
-        <v>51</v>
-      </c>
-      <c r="G64" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="H64" s="33" t="s">
-        <v>146</v>
+        <v>87</v>
+      </c>
+      <c r="G64" s="29"/>
+      <c r="H64" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="B65">
-        <v>37.47</v>
+        <v>123.19</v>
       </c>
       <c r="C65">
-        <v>78.099999999999994</v>
+        <v>22.23</v>
       </c>
       <c r="D65">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="E65" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="F65" t="s">
-        <v>51</v>
-      </c>
-      <c r="G65" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="H65" s="33" t="s">
-        <v>146</v>
+        <v>87</v>
+      </c>
+      <c r="G65" s="29"/>
+      <c r="H65" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="B66">
-        <v>38.1</v>
+        <v>24.13</v>
       </c>
       <c r="C66">
-        <v>27.94</v>
+        <v>91.44</v>
       </c>
       <c r="D66">
         <v>90</v>
       </c>
       <c r="E66" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="F66" t="s">
-        <v>51</v>
-      </c>
-      <c r="G66" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="H66" s="33" t="s">
-        <v>146</v>
+        <v>95</v>
+      </c>
+      <c r="G66" s="30"/>
+      <c r="H66" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>137</v>
+        <v>96</v>
       </c>
       <c r="B67">
-        <v>37.21</v>
+        <v>123.19</v>
       </c>
       <c r="C67">
-        <v>44.2</v>
+        <v>50.17</v>
       </c>
       <c r="D67">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="E67" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="F67" t="s">
-        <v>51</v>
-      </c>
-      <c r="G67" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="H67" s="33" t="s">
-        <v>146</v>
+        <v>87</v>
+      </c>
+      <c r="G67" s="30"/>
+      <c r="H67" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>97</v>
       </c>
       <c r="B68">
-        <v>130.81</v>
+        <v>6.99</v>
       </c>
       <c r="C68">
-        <v>40.64</v>
+        <v>62.23</v>
       </c>
       <c r="D68">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="E68" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="F68" t="s">
-        <v>51</v>
-      </c>
-      <c r="G68" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="H68" s="33" t="s">
-        <v>146</v>
+        <v>99</v>
+      </c>
+      <c r="G68" s="31"/>
+      <c r="H68" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
       <c r="B69">
-        <v>130.81</v>
+        <v>123.19</v>
       </c>
       <c r="C69">
-        <v>70.48</v>
+        <v>76.2</v>
       </c>
       <c r="D69">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="E69" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="F69" t="s">
-        <v>51</v>
-      </c>
-      <c r="G69" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="H69" s="33" t="s">
-        <v>146</v>
+        <v>87</v>
+      </c>
+      <c r="G69" s="32"/>
+      <c r="H69" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="B70">
-        <v>128.91</v>
+        <v>6.99</v>
       </c>
       <c r="C70">
-        <v>93.98</v>
+        <v>48.26</v>
       </c>
       <c r="D70">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E70" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="F70" t="s">
-        <v>51</v>
-      </c>
-      <c r="G70" s="45" t="s">
-        <v>123</v>
-      </c>
-      <c r="H70" s="33" t="s">
-        <v>146</v>
+        <v>99</v>
+      </c>
+      <c r="G70" s="33"/>
+      <c r="H70" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="B71">
-        <v>43.82</v>
+        <v>-14.54</v>
       </c>
       <c r="C71">
-        <v>76.2</v>
+        <v>81.92</v>
       </c>
       <c r="D71">
         <v>270</v>
       </c>
       <c r="E71" t="s">
-        <v>86</v>
-      </c>
-      <c r="F71" t="s">
-        <v>87</v>
-      </c>
-      <c r="G71" s="46" t="s">
-        <v>86</v>
-      </c>
-      <c r="H71" s="33" t="s">
-        <v>146</v>
+        <v>123</v>
+      </c>
+      <c r="G71" s="34"/>
+      <c r="H71" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="B72">
-        <v>43.82</v>
+        <v>41.28</v>
       </c>
       <c r="C72">
-        <v>43.81</v>
+        <v>84.45</v>
       </c>
       <c r="D72">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="E72" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="F72" t="s">
-        <v>87</v>
-      </c>
-      <c r="G72" s="47" t="s">
-        <v>86</v>
-      </c>
-      <c r="H72" s="33" t="s">
-        <v>146</v>
+        <v>10</v>
+      </c>
+      <c r="G72" s="35"/>
+      <c r="H72" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="B73">
-        <v>123.19</v>
+        <v>41.28</v>
       </c>
       <c r="C73">
-        <v>35.56</v>
+        <v>53.98</v>
       </c>
       <c r="D73">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="E73" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="F73" t="s">
-        <v>87</v>
-      </c>
-      <c r="G73" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="H73" s="33" t="s">
-        <v>146</v>
+        <v>10</v>
+      </c>
+      <c r="G73" s="36"/>
+      <c r="H73" s="21" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
       <c r="B74">
-        <v>123.19</v>
+        <v>126.37</v>
       </c>
       <c r="C74">
-        <v>63.5</v>
+        <v>29.21</v>
       </c>
       <c r="D74">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E74" t="s">
-        <v>86</v>
+        <v>14</v>
       </c>
       <c r="F74" t="s">
-        <v>87</v>
-      </c>
-      <c r="G74" s="49" t="s">
-        <v>86</v>
-      </c>
-      <c r="H74" s="33" t="s">
-        <v>146</v>
+        <v>10</v>
+      </c>
+      <c r="G74" s="37"/>
+      <c r="H74" s="21" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
       <c r="B75">
+        <v>126.37</v>
+      </c>
+      <c r="C75">
+        <v>57.15</v>
+      </c>
+      <c r="D75">
+        <v>180</v>
+      </c>
+      <c r="E75" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75" t="s">
+        <v>10</v>
+      </c>
+      <c r="G75" s="39"/>
+      <c r="H75" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>109</v>
+      </c>
+      <c r="B76">
+        <v>126.37</v>
+      </c>
+      <c r="C76">
+        <v>82.55</v>
+      </c>
+      <c r="D76">
+        <v>180</v>
+      </c>
+      <c r="E76" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76" t="s">
+        <v>10</v>
+      </c>
+      <c r="H76" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>139</v>
+      </c>
+      <c r="B77">
+        <v>-6.22</v>
+      </c>
+      <c r="C77">
+        <v>81.28</v>
+      </c>
+      <c r="D77">
+        <v>270</v>
+      </c>
+      <c r="E77" t="s">
+        <v>140</v>
+      </c>
+      <c r="F77" t="s">
+        <v>141</v>
+      </c>
+      <c r="H77" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>142</v>
+      </c>
+      <c r="B78">
+        <v>-4.57</v>
+      </c>
+      <c r="C78">
+        <v>90.55</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>140</v>
+      </c>
+      <c r="F78" t="s">
+        <v>141</v>
+      </c>
+      <c r="H78" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>110</v>
+      </c>
+      <c r="B79">
+        <v>37.47</v>
+      </c>
+      <c r="C79">
+        <v>64.77</v>
+      </c>
+      <c r="D79">
+        <v>90</v>
+      </c>
+      <c r="E79" t="s">
+        <v>73</v>
+      </c>
+      <c r="F79" t="s">
+        <v>51</v>
+      </c>
+      <c r="H79" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>111</v>
+      </c>
+      <c r="B80">
+        <v>37.47</v>
+      </c>
+      <c r="C80">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="D80">
+        <v>90</v>
+      </c>
+      <c r="E80" t="s">
+        <v>73</v>
+      </c>
+      <c r="F80" t="s">
+        <v>51</v>
+      </c>
+      <c r="H80" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>112</v>
+      </c>
+      <c r="B81">
+        <v>38.1</v>
+      </c>
+      <c r="C81">
+        <v>27.94</v>
+      </c>
+      <c r="D81">
+        <v>90</v>
+      </c>
+      <c r="E81" t="s">
+        <v>73</v>
+      </c>
+      <c r="F81" t="s">
+        <v>51</v>
+      </c>
+      <c r="H81" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82">
+        <v>37.21</v>
+      </c>
+      <c r="C82">
+        <v>44.2</v>
+      </c>
+      <c r="D82">
+        <v>90</v>
+      </c>
+      <c r="E82" t="s">
+        <v>73</v>
+      </c>
+      <c r="F82" t="s">
+        <v>51</v>
+      </c>
+      <c r="H82" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>114</v>
+      </c>
+      <c r="B83">
+        <v>130.81</v>
+      </c>
+      <c r="C83">
+        <v>40.64</v>
+      </c>
+      <c r="D83">
+        <v>270</v>
+      </c>
+      <c r="E83" t="s">
+        <v>73</v>
+      </c>
+      <c r="F83" t="s">
+        <v>51</v>
+      </c>
+      <c r="H83" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>115</v>
+      </c>
+      <c r="B84">
+        <v>130.81</v>
+      </c>
+      <c r="C84">
+        <v>70.48</v>
+      </c>
+      <c r="D84">
+        <v>90</v>
+      </c>
+      <c r="E84" t="s">
+        <v>73</v>
+      </c>
+      <c r="F84" t="s">
+        <v>51</v>
+      </c>
+      <c r="H84" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>116</v>
+      </c>
+      <c r="B85">
+        <v>128.91</v>
+      </c>
+      <c r="C85">
+        <v>93.98</v>
+      </c>
+      <c r="D85">
+        <v>90</v>
+      </c>
+      <c r="E85" t="s">
+        <v>73</v>
+      </c>
+      <c r="F85" t="s">
+        <v>51</v>
+      </c>
+      <c r="H85" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>117</v>
+      </c>
+      <c r="B86">
+        <v>43.82</v>
+      </c>
+      <c r="C86">
+        <v>76.2</v>
+      </c>
+      <c r="D86">
+        <v>270</v>
+      </c>
+      <c r="E86" t="s">
+        <v>86</v>
+      </c>
+      <c r="F86" t="s">
+        <v>87</v>
+      </c>
+      <c r="H86" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>118</v>
+      </c>
+      <c r="B87">
+        <v>43.82</v>
+      </c>
+      <c r="C87">
+        <v>43.81</v>
+      </c>
+      <c r="D87">
+        <v>270</v>
+      </c>
+      <c r="E87" t="s">
+        <v>86</v>
+      </c>
+      <c r="F87" t="s">
+        <v>87</v>
+      </c>
+      <c r="H87" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>119</v>
+      </c>
+      <c r="B88">
         <v>123.19</v>
       </c>
-      <c r="C75">
+      <c r="C88">
+        <v>35.56</v>
+      </c>
+      <c r="D88">
+        <v>90</v>
+      </c>
+      <c r="E88" t="s">
+        <v>86</v>
+      </c>
+      <c r="F88" t="s">
+        <v>87</v>
+      </c>
+      <c r="H88" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>120</v>
+      </c>
+      <c r="B89">
+        <v>123.19</v>
+      </c>
+      <c r="C89">
+        <v>63.5</v>
+      </c>
+      <c r="D89">
+        <v>90</v>
+      </c>
+      <c r="E89" t="s">
+        <v>86</v>
+      </c>
+      <c r="F89" t="s">
+        <v>87</v>
+      </c>
+      <c r="H89" s="21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>121</v>
+      </c>
+      <c r="B90">
+        <v>123.19</v>
+      </c>
+      <c r="C90">
         <v>89.54</v>
       </c>
-      <c r="D75">
+      <c r="D90">
         <v>90</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E90" t="s">
         <v>86</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F90" t="s">
         <v>87</v>
       </c>
-      <c r="G75" s="51" t="s">
-        <v>86</v>
-      </c>
-      <c r="H75" s="33" t="s">
-        <v>146</v>
+      <c r="H90" s="21" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>